<commit_message>
EPBDS-12254 ClassCastException in Rule Services if external SpreadsheetResult is returned.
</commit_message>
<xml_diff>
--- a/STUDIO/org.openl.rules.test/test-resources/functionality/EPBDS-11038_Test_Precision/Module1.xlsx
+++ b/STUDIO/org.openl.rules.test/test-resources/functionality/EPBDS-11038_Test_Precision/Module1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\work\demo\openl-demo\user-workspace\DEFAULT\Universal Life Rater\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\openl-tablets\STUDIO\org.openl.rules.test\test-resources\functionality\EPBDS-11038_Test_Precision\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1ED04F5-2014-47EB-B88F-EF4318522F05}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D3A51D0-3C33-4931-A8AD-BEA05580AE56}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="805" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="18770" yWindow="1500" windowWidth="18280" windowHeight="14230" tabRatio="805" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="5" r:id="rId1"/>
@@ -26,6 +26,8 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -57,9 +59,6 @@
   </si>
   <si>
     <t>MyParam</t>
-  </si>
-  <si>
-    <t>= new SpreadsheetResult[] {new SpreadsheetResult(), new SpreadsheetResult()}</t>
   </si>
   <si>
     <t>Spreadsheet SpreadsheetResult CalculateFinalStepRates ( SpreadsheetResult slope)</t>
@@ -203,6 +202,9 @@
   </si>
   <si>
     <t>12</t>
+  </si>
+  <si>
+    <t>= new SpreadsheetResult[] {new SpreadsheetResult(), new SpreadsheetResult()}</t>
   </si>
 </sst>
 </file>
@@ -773,24 +775,24 @@
       <selection activeCell="C15" sqref="C15:E19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="13.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="7.42578125" style="26" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="13.140625" style="26" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="35.5703125" style="26" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="87.85546875" style="26" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="8.85546875" style="26" collapsed="1"/>
-    <col min="6" max="6" width="8.140625" style="26" customWidth="1" collapsed="1"/>
-    <col min="7" max="16384" width="8.85546875" style="26" collapsed="1"/>
+    <col min="1" max="1" width="7.453125" style="26" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="13.1796875" style="26" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="35.54296875" style="26" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="87.81640625" style="26" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="8.81640625" style="26" collapsed="1"/>
+    <col min="6" max="6" width="8.1796875" style="26" customWidth="1" collapsed="1"/>
+    <col min="7" max="16384" width="8.81640625" style="26" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:7" x14ac:dyDescent="0.35">
       <c r="C3" s="51" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D3" s="51"/>
     </row>
-    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:7" x14ac:dyDescent="0.35">
       <c r="C4" s="18" t="s">
         <v>0</v>
       </c>
@@ -798,27 +800,27 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:7" x14ac:dyDescent="0.35">
       <c r="C5" s="37" t="s">
         <v>6</v>
       </c>
       <c r="D5" s="31" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="2:7" x14ac:dyDescent="0.35">
       <c r="D6" s="8"/>
     </row>
-    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:7" x14ac:dyDescent="0.35">
       <c r="D7" s="8"/>
     </row>
-    <row r="8" spans="2:7" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:7" ht="30.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C8" s="52" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D8" s="52"/>
     </row>
-    <row r="9" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:7" x14ac:dyDescent="0.35">
       <c r="C9" s="20" t="s">
         <v>0</v>
       </c>
@@ -827,176 +829,176 @@
       </c>
       <c r="G9" s="28"/>
     </row>
-    <row r="10" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B10" s="27"/>
       <c r="C10" s="45" t="s">
         <v>4</v>
       </c>
       <c r="D10" s="31" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G10" s="28"/>
     </row>
-    <row r="11" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B11" s="27"/>
       <c r="C11" s="45"/>
       <c r="D11" s="31"/>
       <c r="G11" s="28"/>
     </row>
-    <row r="15" spans="2:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:7" ht="14.5" x14ac:dyDescent="0.35">
       <c r="C15" s="48" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D15" s="25"/>
       <c r="E15" s="25"/>
     </row>
-    <row r="16" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:7" x14ac:dyDescent="0.35">
       <c r="C16" s="49" t="s">
+        <v>19</v>
+      </c>
+      <c r="D16" s="49" t="s">
         <v>20</v>
-      </c>
-      <c r="D16" s="49" t="s">
-        <v>21</v>
       </c>
       <c r="E16" s="49">
         <v>3</v>
       </c>
     </row>
-    <row r="17" spans="3:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="17" spans="3:5" ht="14.5" x14ac:dyDescent="0.35">
       <c r="C17" s="25" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D17" s="25" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E17" s="25"/>
     </row>
-    <row r="18" spans="3:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="18" spans="3:5" ht="14.5" x14ac:dyDescent="0.35">
       <c r="C18" s="25" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D18" s="50" t="s">
         <v>7</v>
       </c>
       <c r="E18" s="25"/>
     </row>
-    <row r="19" spans="3:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="19" spans="3:5" ht="14.5" x14ac:dyDescent="0.35">
       <c r="C19" s="25" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D19" s="25" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E19" s="25"/>
     </row>
-    <row r="20" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C20" s="3"/>
       <c r="D20" s="3"/>
       <c r="E20" s="3"/>
     </row>
-    <row r="21" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C21" s="3"/>
       <c r="D21" s="3"/>
       <c r="E21" s="3"/>
     </row>
-    <row r="22" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C22" s="3"/>
       <c r="D22" s="3"/>
       <c r="E22" s="3"/>
     </row>
-    <row r="23" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C23" s="3"/>
       <c r="D23" s="3"/>
       <c r="E23" s="3"/>
     </row>
-    <row r="24" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C24" s="3"/>
       <c r="D24" s="3"/>
       <c r="E24" s="3"/>
     </row>
-    <row r="25" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C25" s="3"/>
       <c r="D25" s="3"/>
       <c r="E25" s="3"/>
     </row>
-    <row r="26" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C26" s="3"/>
       <c r="D26" s="3"/>
       <c r="E26" s="3"/>
     </row>
-    <row r="27" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C27" s="3"/>
       <c r="D27" s="3"/>
       <c r="E27" s="3"/>
     </row>
-    <row r="28" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C28" s="3"/>
       <c r="D28" s="3"/>
       <c r="E28" s="3"/>
     </row>
-    <row r="29" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C29" s="3"/>
       <c r="D29" s="3"/>
       <c r="E29" s="3"/>
     </row>
-    <row r="30" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C30" s="3"/>
       <c r="D30" s="3"/>
       <c r="E30" s="3"/>
     </row>
-    <row r="31" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C31" s="3"/>
       <c r="D31" s="3"/>
       <c r="E31" s="3"/>
     </row>
-    <row r="32" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C32" s="3"/>
       <c r="D32" s="3"/>
       <c r="E32" s="3"/>
     </row>
-    <row r="33" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C33" s="3"/>
       <c r="D33" s="3"/>
       <c r="E33" s="3"/>
     </row>
-    <row r="34" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C34" s="3"/>
       <c r="D34" s="3"/>
       <c r="E34" s="3"/>
     </row>
-    <row r="36" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C36" s="16"/>
       <c r="D36" s="44"/>
     </row>
-    <row r="37" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C37" s="16"/>
       <c r="D37" s="43"/>
     </row>
-    <row r="38" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C38" s="16"/>
       <c r="D38" s="44"/>
     </row>
-    <row r="56" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="56" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C56" s="16"/>
       <c r="D56" s="43"/>
     </row>
-    <row r="57" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="57" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C57" s="16"/>
       <c r="D57" s="43"/>
     </row>
-    <row r="58" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="58" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C58" s="16"/>
       <c r="D58" s="43"/>
     </row>
-    <row r="59" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="59" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C59" s="16"/>
       <c r="D59" s="43"/>
       <c r="F59" s="10"/>
     </row>
-    <row r="60" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="60" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C60" s="16"/>
       <c r="D60" s="43"/>
     </row>
-    <row r="61" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="61" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C61" s="16"/>
       <c r="D61" s="43"/>
     </row>
@@ -1019,30 +1021,30 @@
       <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="3" max="3" width="24.42578125" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="110.28515625" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="24.453125" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="110.26953125" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A2" s="2"/>
       <c r="B2" s="2"/>
       <c r="C2" s="5"/>
       <c r="D2" s="7"/>
     </row>
-    <row r="3" spans="1:10" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" ht="30.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="2"/>
       <c r="B3" s="2"/>
       <c r="C3" s="53" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D3" s="53"/>
       <c r="H3" s="25"/>
       <c r="I3" s="25"/>
       <c r="J3" s="25"/>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A4" s="2"/>
       <c r="B4" s="2"/>
       <c r="C4" s="19" t="s">
@@ -1055,20 +1057,20 @@
       <c r="I4" s="25"/>
       <c r="J4" s="25"/>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A5" s="2"/>
       <c r="B5" s="2"/>
       <c r="C5" s="42" t="s">
         <v>5</v>
       </c>
       <c r="D5" s="41" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H5" s="25"/>
       <c r="I5" s="25"/>
       <c r="J5" s="25"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A6" s="2"/>
       <c r="B6" s="2"/>
       <c r="C6" s="22"/>
@@ -1078,23 +1080,23 @@
       <c r="I6" s="25"/>
       <c r="J6" s="25"/>
     </row>
-    <row r="7" spans="1:10" s="25" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" s="25" customFormat="1" x14ac:dyDescent="0.35">
       <c r="C7" s="34"/>
     </row>
-    <row r="8" spans="1:10" s="25" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" s="25" customFormat="1" x14ac:dyDescent="0.35">
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
     </row>
-    <row r="9" spans="1:10" s="25" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="10" spans="1:10" s="25" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="11" spans="1:10" s="25" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="12" spans="1:10" s="25" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="13" spans="1:10" s="25" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="14" spans="1:10" s="25" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" s="25" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="10" spans="1:10" s="25" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="11" spans="1:10" s="25" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="12" spans="1:10" s="25" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="13" spans="1:10" s="25" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="14" spans="1:10" s="25" customFormat="1" x14ac:dyDescent="0.35">
       <c r="C14" s="5"/>
       <c r="D14" s="6"/>
     </row>
-    <row r="15" spans="1:10" s="25" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="15" spans="1:10" s="25" customFormat="1" x14ac:dyDescent="0.35"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="C3:D3"/>
@@ -1112,28 +1114,28 @@
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="13.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="8.85546875" style="1" collapsed="1"/>
-    <col min="2" max="2" width="10.5703125" style="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="26.42578125" style="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="8.81640625" style="1" collapsed="1"/>
+    <col min="2" max="2" width="10.54296875" style="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="26.453125" style="1" customWidth="1" collapsed="1"/>
     <col min="4" max="4" width="123" style="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="8.85546875" style="1" collapsed="1"/>
-    <col min="6" max="6" width="8.85546875" style="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="8" width="8.85546875" style="1" collapsed="1"/>
-    <col min="9" max="9" width="18.140625" style="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="101.5703125" style="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="16384" width="8.85546875" style="1" collapsed="1"/>
+    <col min="5" max="5" width="8.81640625" style="1" collapsed="1"/>
+    <col min="6" max="6" width="8.81640625" style="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="8" width="8.81640625" style="1" collapsed="1"/>
+    <col min="9" max="9" width="18.1796875" style="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="101.54296875" style="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="16384" width="8.81640625" style="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
       <c r="D1" s="54"/>
       <c r="E1" s="54"/>
     </row>
-    <row r="3" spans="1:13" ht="27.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" ht="27.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="2"/>
       <c r="C3" s="55" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D3" s="55"/>
       <c r="G3" s="9"/>
@@ -1141,7 +1143,7 @@
       <c r="I3" s="14"/>
       <c r="J3" s="2"/>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A4" s="2"/>
       <c r="C4" s="19" t="s">
         <v>0</v>
@@ -1153,14 +1155,14 @@
       <c r="H4" s="13"/>
       <c r="I4" s="13"/>
     </row>
-    <row r="5" spans="1:13" s="26" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" s="26" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A5" s="15"/>
       <c r="B5" s="27"/>
       <c r="C5" s="29" t="s">
         <v>3</v>
       </c>
       <c r="D5" s="38" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E5" s="27"/>
       <c r="F5" s="35"/>
@@ -1172,7 +1174,7 @@
       <c r="L5" s="27"/>
       <c r="M5" s="27"/>
     </row>
-    <row r="6" spans="1:13" s="26" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" s="26" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A6" s="15"/>
       <c r="B6" s="27"/>
       <c r="C6" s="29"/>
@@ -1187,25 +1189,25 @@
       <c r="L6" s="27"/>
       <c r="M6" s="27"/>
     </row>
-    <row r="7" spans="1:13" s="26" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" s="26" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H7" s="40"/>
       <c r="I7" s="40"/>
       <c r="J7" s="40"/>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.35">
       <c r="H8" s="40"/>
       <c r="I8" s="40"/>
       <c r="J8" s="40"/>
     </row>
-    <row r="9" spans="1:13" s="40" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" s="40" customFormat="1" x14ac:dyDescent="0.35">
       <c r="C9" s="26"/>
       <c r="D9" s="26"/>
     </row>
-    <row r="10" spans="1:13" s="26" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" s="26" customFormat="1" x14ac:dyDescent="0.35">
       <c r="C10" s="5"/>
       <c r="D10" s="6"/>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A11" s="24"/>
     </row>
   </sheetData>
@@ -1223,27 +1225,27 @@
   <dimension ref="A3:F16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17:E29"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="13.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="5" style="26" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="6.5703125" style="26" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="27.5703125" style="26" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="94.85546875" style="26" customWidth="1" collapsed="1"/>
-    <col min="5" max="16384" width="8.85546875" style="26" collapsed="1"/>
+    <col min="2" max="2" width="6.54296875" style="26" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="27.54296875" style="26" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="94.81640625" style="26" customWidth="1" collapsed="1"/>
+    <col min="5" max="16384" width="8.81640625" style="26" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:6" s="25" customFormat="1" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" s="25" customFormat="1" ht="30.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="26"/>
       <c r="C3" s="52" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D3" s="52"/>
       <c r="F3" s="46"/>
     </row>
-    <row r="4" spans="1:6" s="25" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" s="25" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
       <c r="C4" s="33" t="s">
         <v>0</v>
       </c>
@@ -1251,47 +1253,47 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:6" s="25" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" s="25" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
       <c r="C5" s="36" t="s">
         <v>2</v>
       </c>
       <c r="D5" s="39" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" s="25" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" s="25" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
       <c r="C6" s="36" t="s">
         <v>3</v>
       </c>
       <c r="D6" s="11" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" s="25" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" s="25" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
       <c r="C7" s="36"/>
       <c r="D7" s="30"/>
     </row>
-    <row r="8" spans="1:6" s="25" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" s="25" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
       <c r="D8" s="47"/>
     </row>
-    <row r="9" spans="1:6" s="25" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" s="25" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
       <c r="D9" s="47"/>
     </row>
-    <row r="10" spans="1:6" s="25" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" s="25" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
       <c r="C10" s="16"/>
       <c r="D10" s="17"/>
     </row>
-    <row r="11" spans="1:6" s="25" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" s="25" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
       <c r="C11" s="26"/>
       <c r="D11" s="26"/>
     </row>
-    <row r="12" spans="1:6" s="25" customFormat="1" ht="29.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" s="25" customFormat="1" ht="29.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C12" s="52" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D12" s="52"/>
     </row>
-    <row r="13" spans="1:6" s="25" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" s="25" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
       <c r="C13" s="33" t="s">
         <v>0</v>
       </c>
@@ -1299,7 +1301,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:6" s="25" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" s="25" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
       <c r="C14" s="36" t="s">
         <v>7</v>
       </c>
@@ -1308,8 +1310,8 @@
         <v>6.4444440000000006E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:6" s="25" customFormat="1" ht="15" x14ac:dyDescent="0.25"/>
-    <row r="16" spans="1:6" s="25" customFormat="1" ht="15" x14ac:dyDescent="0.25"/>
+    <row r="15" spans="1:6" s="25" customFormat="1" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="16" spans="1:6" s="25" customFormat="1" ht="14.5" x14ac:dyDescent="0.35"/>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="C3:D3"/>

</xml_diff>